<commit_message>
Formatting tables 4.3.6, 4.3.15
</commit_message>
<xml_diff>
--- a/tests/manual/integration/4.3.15.ConfiguratorMSHK-01.DefaultValues.PageReloading.xlsx
+++ b/tests/manual/integration/4.3.15.ConfiguratorMSHK-01.DefaultValues.PageReloading.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pa\art\tests\manual\integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9E7D10-CC27-4F55-83A8-74300DA74B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB358814-A498-494B-942B-729A83871AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="sourses" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,55 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
-  <si>
-    <t>Модуль</t>
-  </si>
-  <si>
-    <t>Предусловия</t>
-  </si>
-  <si>
-    <t>Шаги</t>
-  </si>
-  <si>
-    <t>Ожидаемый результат</t>
-  </si>
-  <si>
-    <t>Номер</t>
-  </si>
-  <si>
-    <t>Статус</t>
-  </si>
-  <si>
-    <t>Заголовок</t>
-  </si>
-  <si>
-    <t>Конфигуратор МШК-01</t>
-  </si>
-  <si>
-    <t>Проверка значений по умолчанию
-после перезагрузки страницы</t>
-  </si>
-  <si>
-    <t>1. Проверить значение в поле "Механизм"</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>Поле "Механизм" имеет значение
 "МШК-01"</t>
   </si>
   <si>
-    <t>2. Проверить значение в поле выбора "Отдельно стоящий"</t>
-  </si>
-  <si>
-    <t>3. Проверить значение в поле выбора "Механизм дивана"</t>
-  </si>
-  <si>
-    <t>4. Проверить значение в поле выбора "Глубина дивана"</t>
-  </si>
-  <si>
-    <t>5. Проверить значение в поле выбора "Глубина механизма"</t>
-  </si>
-  <si>
     <t>Поле выбора "Глубина механизма" имеет
 значение "430"</t>
   </si>
@@ -90,15 +48,6 @@
 значение "ОС"</t>
   </si>
   <si>
-    <t>8. Проверить значение в поле ввода "Длина спального места"</t>
-  </si>
-  <si>
-    <t>7. Проверить значение в поле ввода "Ширина спального места"</t>
-  </si>
-  <si>
-    <t>6. Проверить значение в поле ввода "Глубина шкафа"</t>
-  </si>
-  <si>
     <t>Поле ввода "Глубина шкафа" имеет
 значение "430"</t>
   </si>
@@ -109,34 +58,16 @@
     <t>Поле ввода "Длина спального места" имеет значение "2000"</t>
   </si>
   <si>
-    <t>9. Проверить значение в поле выбора "Опоры"</t>
-  </si>
-  <si>
     <t>Поле выбора "Опоры" имеет значение "ОК"</t>
   </si>
   <si>
-    <t>10. Проверить значение в поле выбора "Высота опор"</t>
-  </si>
-  <si>
     <t>Поле выбора "Высота опор" имеет значение "250"</t>
   </si>
   <si>
-    <t>11. Проверить значение в поле выбора "Высота оси вращения"</t>
-  </si>
-  <si>
-    <t>12. Проверить значение в поле выбора "Усиленное исполнение"</t>
-  </si>
-  <si>
     <t>Поле выбора "Усиленное исполнение" имеет значение "НЕТ"</t>
   </si>
   <si>
-    <t>13. Проверить значение в поле выбора "Фиксация фасада"</t>
-  </si>
-  <si>
     <t>Поле выбора "Фиксация фасада" имеет значение "КН"</t>
-  </si>
-  <si>
-    <t>14. Проверить значение в поле выбора "Электродвигатель"</t>
   </si>
   <si>
     <t>Поле выбора "Электродвигатель" имеет значение "НЕТ"</t>
@@ -144,6 +75,102 @@
   <si>
     <t>1. Страница МШК-01 перезагружена
 2. Конфигуратор МШК-01 в видимой области окна браузера</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Hight</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Skipped</t>
+  </si>
+  <si>
+    <t>No run</t>
+  </si>
+  <si>
+    <t>Blocked</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Precondition</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Test data</t>
+  </si>
+  <si>
+    <t>Expected result</t>
+  </si>
+  <si>
+    <t>Проверить значение в поле "Механизм"</t>
+  </si>
+  <si>
+    <t>Проверить значение в поле выбора "Отдельно стоящий"</t>
+  </si>
+  <si>
+    <t>Проверить значение в поле выбора "Механизм дивана"</t>
+  </si>
+  <si>
+    <t>Проверить значение в поле выбора "Глубина дивана"</t>
+  </si>
+  <si>
+    <t>Проверить значение в поле выбора "Глубина механизма"</t>
+  </si>
+  <si>
+    <t>Проверить значение в поле ввода "Глубина шкафа"</t>
+  </si>
+  <si>
+    <t>Проверить значение в поле ввода "Ширина спального места"</t>
+  </si>
+  <si>
+    <t>Проверить значение в поле ввода "Длина спального места"</t>
+  </si>
+  <si>
+    <t>Проверить значение в поле выбора "Опоры"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Проверить значение в поле выбора "Высота опор"</t>
+  </si>
+  <si>
+    <t>Проверить значение в поле выбора "Высота оси вращения"</t>
+  </si>
+  <si>
+    <t>Проверить значение в поле выбора "Усиленное исполнение"</t>
+  </si>
+  <si>
+    <t>Проверить значение в поле выбора "Фиксация фасада"</t>
+  </si>
+  <si>
+    <t>Проверить значение в поле выбора "Электродвигатель"</t>
+  </si>
+  <si>
+    <t>Проверка значений по умолчанию после перезагрузки страницы</t>
   </si>
 </sst>
 </file>
@@ -168,7 +195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +205,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -209,25 +242,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -543,237 +576,329 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="39.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="4.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="39.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="42.5546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="42.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="I3" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5">
+        <v>5</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="F7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="I7" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5">
         <v>7</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="F8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5">
         <v>8</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="F9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5">
         <v>10</v>
       </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="3" t="s">
+      <c r="F11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5">
         <v>11</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="3" t="s">
+      <c r="F12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5">
         <v>12</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="3" t="s">
+      <c r="F13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5">
         <v>13</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="3" t="s">
+      <c r="F14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5">
         <v>14</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="2"/>
+      <c r="F15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -784,5 +909,82 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8ACF84A6-66A6-4C36-A55E-19D1869C3DDE}">
+          <x14:formula1>
+            <xm:f>sourses!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B15</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B8404B35-06F2-4D17-AC90-9FC6B82D29F9}">
+          <x14:formula1>
+            <xm:f>sourses!$B$2:$B$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I15</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5F233F-54B8-44AE-83FF-620FCB4A01D2}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>